<commit_message>
Fixed models & admin panel. Finished auto-fill DB commands.
</commit_message>
<xml_diff>
--- a/backend/basic_data.xlsx
+++ b/backend/basic_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\VS Code Projects\silant_diploma\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775EFE23-85A9-438A-B4E5-53E83C61353D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DE06D1-859B-49BA-B692-849F87227257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="machines" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="200">
   <si>
     <t>ОБЩИЕ СВЕДЕНИЯ</t>
   </si>
@@ -318,9 +318,6 @@
     <t>АО "Зандер"</t>
   </si>
   <si>
-    <t>АО Зандер</t>
-  </si>
-  <si>
     <t>г. Краснодар</t>
   </si>
   <si>
@@ -383,9 +380,6 @@
     <t>1. Кабина с отопителем;</t>
   </si>
   <si>
-    <t>Зав. № машины</t>
-  </si>
-  <si>
     <t>Вид ТО</t>
   </si>
   <si>
@@ -393,12 +387,6 @@
   </si>
   <si>
     <t>Наработка, м/час</t>
-  </si>
-  <si>
-    <t>№ заказ-наряда</t>
-  </si>
-  <si>
-    <t>дата заказ-наряда</t>
   </si>
   <si>
     <t>Организация, проводившая ТО</t>
@@ -654,6 +642,12 @@
   </si>
   <si>
     <t>Модель трансмиссии</t>
+  </si>
+  <si>
+    <t>Номер заказ-наряда</t>
+  </si>
+  <si>
+    <t>Дата заказ-наряда</t>
   </si>
 </sst>
 </file>
@@ -1134,9 +1128,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1220,52 +1214,52 @@
     </row>
     <row r="3" spans="1:26" ht="60.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>3</v>
@@ -1755,13 +1749,13 @@
         <v>91</v>
       </c>
       <c r="N11" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="O11" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="O11" s="11" t="s">
+      <c r="P11" s="15" t="s">
         <v>93</v>
-      </c>
-      <c r="P11" s="15" t="s">
-        <v>94</v>
       </c>
       <c r="Q11" s="9" t="s">
         <v>17</v>
@@ -1784,31 +1778,31 @@
         <v>18</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>24</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>26</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L12" s="13">
         <v>44589</v>
@@ -1817,16 +1811,16 @@
         <v>28</v>
       </c>
       <c r="N12" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="O12" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="O12" s="17" t="s">
+      <c r="P12" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="P12" s="15" t="s">
+      <c r="Q12" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>103</v>
       </c>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
@@ -1846,31 +1840,31 @@
         <v>42</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>46</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>48</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>50</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L13" s="13">
         <v>44469</v>
@@ -1879,16 +1873,16 @@
         <v>69</v>
       </c>
       <c r="N13" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P13" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O13" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="P13" s="14" t="s">
-        <v>110</v>
-      </c>
       <c r="Q13" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
@@ -29552,7 +29546,9 @@
   </sheetPr>
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -29567,25 +29563,25 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30">
       <c r="A1" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>113</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>117</v>
       </c>
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
@@ -29612,7 +29608,7 @@
         <v>55</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C2" s="21">
         <v>44474</v>
@@ -29621,7 +29617,7 @@
         <v>55</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F2" s="21">
         <v>44472</v>
@@ -29632,10 +29628,10 @@
     </row>
     <row r="3" spans="1:26" ht="12.75">
       <c r="A3" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C3" s="21">
         <v>44474</v>
@@ -29644,13 +29640,13 @@
         <v>54</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F3" s="21">
         <v>44472</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75">
@@ -29658,7 +29654,7 @@
         <v>55</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C4" s="21">
         <v>44502</v>
@@ -29667,7 +29663,7 @@
         <v>220</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F4" s="21">
         <v>44500</v>
@@ -29678,10 +29674,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C5" s="21">
         <v>44502</v>
@@ -29690,13 +29686,13 @@
         <v>225</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F5" s="21">
         <v>44500</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.75">
@@ -29704,7 +29700,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C6" s="21">
         <v>44540</v>
@@ -29713,7 +29709,7 @@
         <v>450</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F6" s="21">
         <v>44538</v>
@@ -29724,10 +29720,10 @@
     </row>
     <row r="7" spans="1:26" ht="12.75">
       <c r="A7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C7" s="21">
         <v>44540</v>
@@ -29736,13 +29732,13 @@
         <v>422</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F7" s="21">
         <v>44538</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75">
@@ -29750,7 +29746,7 @@
         <v>63</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C8" s="21">
         <v>44555</v>
@@ -29759,7 +29755,7 @@
         <v>53</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F8" s="21">
         <v>44553</v>
@@ -29773,7 +29769,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C9" s="21">
         <v>44580</v>
@@ -29782,7 +29778,7 @@
         <v>52</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F9" s="21">
         <v>44578</v>
@@ -29796,7 +29792,7 @@
         <v>63</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C10" s="21">
         <v>44583</v>
@@ -29805,7 +29801,7 @@
         <v>221</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F10" s="21">
         <v>44581</v>
@@ -29816,10 +29812,10 @@
     </row>
     <row r="11" spans="1:26" ht="12.75">
       <c r="A11" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C11" s="21">
         <v>44594</v>
@@ -29828,13 +29824,13 @@
         <v>55</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F11" s="21">
         <v>44592</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12.75">
@@ -29842,7 +29838,7 @@
         <v>55</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C12" s="21">
         <v>44605</v>
@@ -29851,7 +29847,7 @@
         <v>1054</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F12" s="21">
         <v>44603</v>
@@ -29862,10 +29858,10 @@
     </row>
     <row r="13" spans="1:26" ht="12.75">
       <c r="A13" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C13" s="21">
         <v>44605</v>
@@ -29874,13 +29870,13 @@
         <v>1026</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F13" s="21">
         <v>44603</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="12.75">
@@ -29888,7 +29884,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C14" s="21">
         <v>44608</v>
@@ -29897,7 +29893,7 @@
         <v>221</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F14" s="21">
         <v>44606</v>
@@ -29911,7 +29907,7 @@
         <v>63</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C15" s="21">
         <v>44621</v>
@@ -29920,7 +29916,7 @@
         <v>407</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F15" s="21">
         <v>44619</v>
@@ -29931,10 +29927,10 @@
     </row>
     <row r="16" spans="1:26" ht="12.75">
       <c r="A16" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C16" s="21">
         <v>44622</v>
@@ -29943,13 +29939,13 @@
         <v>219</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F16" s="21">
         <v>44620</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="12.75">
@@ -29957,7 +29953,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C17" s="21">
         <v>44634</v>
@@ -29966,13 +29962,13 @@
         <v>53</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F17" s="21">
         <v>44632</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="12.75">
@@ -29980,7 +29976,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C18" s="21">
         <v>44646</v>
@@ -29989,7 +29985,7 @@
         <v>403</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F18" s="21">
         <v>44644</v>
@@ -30000,10 +29996,10 @@
     </row>
     <row r="19" spans="1:7" ht="12.75">
       <c r="A19" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C19" s="21">
         <v>44660</v>
@@ -30012,13 +30008,13 @@
         <v>405</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F19" s="21">
         <v>44658</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75">
@@ -30026,7 +30022,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C20" s="21">
         <v>44662</v>
@@ -30035,13 +30031,13 @@
         <v>210</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F20" s="21">
         <v>44660</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75">
@@ -30049,7 +30045,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C21" s="21">
         <v>44684</v>
@@ -30058,7 +30054,7 @@
         <v>52</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F21" s="21">
         <v>44682</v>
@@ -30072,7 +30068,7 @@
         <v>63</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C22" s="21">
         <v>44686</v>
@@ -30081,13 +30077,13 @@
         <v>1011</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F22" s="21">
         <v>44684</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75">
@@ -30095,7 +30091,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C23" s="21">
         <v>44700</v>
@@ -30104,13 +30100,13 @@
         <v>405</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F23" s="21">
         <v>44698</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75">
@@ -30118,7 +30114,7 @@
         <v>33</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C24" s="21">
         <v>44712</v>
@@ -30127,7 +30123,7 @@
         <v>214</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F24" s="21">
         <v>44710</v>
@@ -30141,7 +30137,7 @@
         <v>43</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C25" s="21">
         <v>44713</v>
@@ -30150,7 +30146,7 @@
         <v>55</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F25" s="21">
         <v>44711</v>
@@ -30164,7 +30160,7 @@
         <v>43</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C26" s="21">
         <v>44741</v>
@@ -30173,7 +30169,7 @@
         <v>216</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F26" s="21">
         <v>44739</v>
@@ -30187,7 +30183,7 @@
         <v>33</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C27" s="21">
         <v>44750</v>
@@ -30196,7 +30192,7 @@
         <v>441</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F27" s="21">
         <v>44748</v>
@@ -30210,7 +30206,7 @@
         <v>73</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C28" s="21">
         <v>44765</v>
@@ -30219,13 +30215,13 @@
         <v>54</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F28" s="21">
         <v>44763</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="12.75">
@@ -30233,7 +30229,7 @@
         <v>43</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C29" s="21">
         <v>44779</v>
@@ -30242,7 +30238,7 @@
         <v>434</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F29" s="21">
         <v>44777</v>
@@ -30256,7 +30252,7 @@
         <v>73</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C30" s="21">
         <v>44793</v>
@@ -30265,13 +30261,13 @@
         <v>206</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F30" s="21">
         <v>44791</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="12.75">
@@ -30279,7 +30275,7 @@
         <v>55</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C31" s="21">
         <v>44805</v>
@@ -30288,7 +30284,7 @@
         <v>2053</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F31" s="21">
         <v>44803</v>
@@ -30299,10 +30295,10 @@
     </row>
     <row r="32" spans="1:7" ht="12.75">
       <c r="A32" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C32" s="21">
         <v>44805</v>
@@ -30311,13 +30307,13 @@
         <v>2025</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F32" s="21">
         <v>44803</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="12.75">
@@ -30325,7 +30321,7 @@
         <v>86</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C33" s="21">
         <v>44808</v>
@@ -30334,13 +30330,13 @@
         <v>53</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F33" s="21">
         <v>44806</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="12.75">
@@ -30348,7 +30344,7 @@
         <v>73</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C34" s="21">
         <v>44831</v>
@@ -30357,13 +30353,13 @@
         <v>407</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F34" s="21">
         <v>44829</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="12.75">
@@ -30371,7 +30367,7 @@
         <v>86</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C35" s="21">
         <v>44836</v>
@@ -30380,13 +30376,13 @@
         <v>202</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F35" s="21">
         <v>44834</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="12.75">
@@ -30394,7 +30390,7 @@
         <v>86</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C36" s="21">
         <v>44874</v>
@@ -30403,13 +30399,13 @@
         <v>402</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F36" s="21">
         <v>44872</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="12.75">
@@ -30417,7 +30413,7 @@
         <v>63</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C37" s="21">
         <v>44886</v>
@@ -30426,13 +30422,13 @@
         <v>2010</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F37" s="21">
         <v>44884</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="12.75">
@@ -30454,7 +30450,9 @@
   </sheetPr>
   <dimension ref="A2:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -30464,31 +30462,31 @@
   <sheetData>
     <row r="2" spans="1:9">
       <c r="A2" s="18" t="s">
-        <v>111</v>
+        <v>189</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>162</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -30502,16 +30500,16 @@
         <v>123</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H3" s="13">
         <v>44659.0625</v>
@@ -30531,16 +30529,16 @@
         <v>129</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F4" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>169</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>173</v>
       </c>
       <c r="H4" s="13">
         <v>44658.1875</v>
@@ -30560,13 +30558,13 @@
         <v>112</v>
       </c>
       <c r="D5" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="27" t="s">
         <v>171</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>175</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="13">
@@ -30587,16 +30585,16 @@
         <v>123</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H6" s="13">
         <v>44603.0625</v>
@@ -30616,16 +30614,16 @@
         <v>38</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H7" s="13">
         <v>44688.125</v>
@@ -30645,16 +30643,16 @@
         <v>112</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H8" s="13">
         <v>44737</v>
@@ -30674,16 +30672,16 @@
         <v>142</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H9" s="13">
         <v>44502.625</v>
@@ -30703,16 +30701,16 @@
         <v>61</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H10" s="13">
         <v>44566.4375</v>
@@ -30732,16 +30730,16 @@
         <v>56</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H11" s="13">
         <v>44774.5</v>
@@ -30761,16 +30759,16 @@
         <v>47</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H12" s="13">
         <v>44813.8125</v>
@@ -30781,7 +30779,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="13">
         <v>44593.125</v>
@@ -30790,13 +30788,13 @@
         <v>22</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="13">
@@ -30808,7 +30806,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="13">
         <v>44480.0625</v>
@@ -30817,16 +30815,16 @@
         <v>59</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H14" s="13">
         <v>44490.0625</v>

</xml_diff>